<commit_message>
se modif de nuevo data para Regresión Preprod 06-05-2021 (se mejoróa data de complementaria, prendario y blanket)
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Emision Motor - Prendario.xlsx
+++ b/Sura/DataSource - Emision Motor - Prendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71891C7-01EB-4C12-9D64-2912305EB8CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EC5C82-B291-4F4F-B2D2-92C47B065A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,13 +179,13 @@
     <t>20/05/2021</t>
   </si>
   <si>
-    <t>RGM013</t>
-  </si>
-  <si>
-    <t>1234567RGM013</t>
-  </si>
-  <si>
-    <t>03/05/2021</t>
+    <t>06/05/2021</t>
+  </si>
+  <si>
+    <t>RGM014</t>
+  </si>
+  <si>
+    <t>1234567RGM014</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:AF17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
     <col min="21" max="21" width="11.5703125" customWidth="1"/>
     <col min="22" max="22" width="22.42578125" customWidth="1"/>
     <col min="23" max="23" width="21.85546875" customWidth="1"/>
-    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="25.7109375" customWidth="1"/>
     <col min="25" max="25" width="17.7109375" customWidth="1"/>
     <col min="26" max="26" width="12.42578125" customWidth="1"/>
     <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
@@ -699,7 +699,7 @@
         <v>23</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="R2">
         <v>2021</v>
@@ -717,13 +717,13 @@
         <v>33</v>
       </c>
       <c r="W2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Y2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Z2" t="s">
         <v>17</v>

</xml_diff>